<commit_message>
Update ig name 27d0eaa3dd564ea8bcfc2f246940a4291853ae4e
</commit_message>
<xml_diff>
--- a/ANS-170-ST/ig/CodeSystem-competence-code-system.xlsx
+++ b/ANS-170-ST/ig/CodeSystem-competence-code-system.xlsx
@@ -24,13 +24,13 @@
     <t>URL</t>
   </si>
   <si>
-    <t>https://interop.esante.gouv.fr/ig/fhir/[code]/CodeSystem/competence-code-system</t>
+    <t>https://interop.esante.gouv.fr/ig/fhir/tde/CodeSystem/competence-code-system</t>
   </si>
   <si>
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.0</t>
+    <t>2.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2026-01-15T13:06:26+00:00</t>
+    <t>2026-01-15T15:23:39+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>